<commit_message>
Update E-Step Calibration Calculator.xlsx
</commit_message>
<xml_diff>
--- a/E-Step Calculator/E-Step Calibration Calculator.xlsx
+++ b/E-Step Calculator/E-Step Calibration Calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicho\OneDrive\3D Printing\GITHUB-QUADMODS\QuadFusion-Mods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicho\OneDrive\3D Printing\GITHUB-QUADMODS\QuadFusion-Mods\E-Step Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="11_55E7BCB05020C167FD3CC87C24DE01DD5A00EE3B" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{635FADCF-432B-4966-B561-8C3A0768C724}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="11_55E7BCB05020C167FD3CC87C24DE01DD5A00EE3B" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{1873A600-D9F6-4739-A3D4-A9C13BB45D42}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="2100" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -532,7 +535,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,21 +547,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -568,7 +571,7 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -576,7 +579,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -586,7 +589,7 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
@@ -662,21 +665,21 @@
         <v>15</v>
       </c>
       <c r="B7" s="6">
-        <v>2186</v>
+        <v>2140</v>
       </c>
       <c r="C7" s="5">
         <v>100</v>
       </c>
       <c r="D7" s="5">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>0.98039215686274506</v>
+        <v>1.0204081632653061</v>
       </c>
       <c r="F7" s="5">
         <f>B7*E7</f>
-        <v>2143.1372549019607</v>
+        <v>2183.6734693877552</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,7 +692,7 @@
       <c r="C8" s="6">
         <v>100</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>99</v>
       </c>
       <c r="E8" s="6">
@@ -711,16 +714,16 @@
       <c r="C9" s="6">
         <v>100</v>
       </c>
-      <c r="D9" s="6">
-        <v>100.5</v>
+      <c r="D9" s="7">
+        <v>97.8</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="2"/>
-        <v>0.99502487562189057</v>
+        <v>1.0224948875255624</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>2129.353233830846</v>
+        <v>2188.1390593047036</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -733,16 +736,16 @@
       <c r="C10" s="6">
         <v>100</v>
       </c>
-      <c r="D10" s="6">
-        <v>100</v>
+      <c r="D10" s="7">
+        <v>103</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.970873786407767</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="3"/>
-        <v>2140</v>
+        <v>2077.6699029126212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated automatic probe locations for my Fan Shroud
</commit_message>
<xml_diff>
--- a/E-Step Calculator/E-Step Calibration Calculator.xlsx
+++ b/E-Step Calculator/E-Step Calibration Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicho\OneDrive\3D Printing\GITHUB-QUADMODS\QuadFusion-Mods\E-Step Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="11_55E7BCB05020C167FD3CC87C24DE01DD5A00EE3B" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{2D802CF3-71EE-40FD-8DE6-07AD0B280099}"/>
+  <xr:revisionPtr revIDLastSave="392" documentId="11_55E7BCB05020C167FD3CC87C24DE01DD5A00EE3B" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{F721B25F-585E-4AD2-948A-30C9DCF081A9}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="2100" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="6">
-        <v>2140</v>
+        <v>2124.8000000000002</v>
       </c>
       <c r="C7" s="5">
         <v>100</v>
@@ -682,7 +682,7 @@
       </c>
       <c r="F7" s="5">
         <f>B7*E7</f>
-        <v>2140</v>
+        <v>2124.8000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,15 +696,15 @@
         <v>100</v>
       </c>
       <c r="D8" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ref="E8:E10" si="2">C8/D8</f>
-        <v>1</v>
+        <v>0.99009900990099009</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ref="F8:F10" si="3">B8*E8</f>
-        <v>2132.9</v>
+        <v>2111.7821782178216</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,15 +718,15 @@
         <v>100</v>
       </c>
       <c r="D9" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.99009900990099009</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>2140.8000000000002</v>
+        <v>2119.6039603960398</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,15 +740,15 @@
         <v>100</v>
       </c>
       <c r="D10" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.99009900990099009</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="3"/>
-        <v>2142.9</v>
+        <v>2121.6831683168316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
micro settings 8 e-steps 1070
</commit_message>
<xml_diff>
--- a/E-Step Calculator/E-Step Calibration Calculator.xlsx
+++ b/E-Step Calculator/E-Step Calibration Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicho\Documents\GitHub\QuadFusion-Mods\E-Step Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F636C43C-3095-4A49-8102-1D6989D7C348}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D5E0F-8F9D-4B27-81D1-29B3F9464079}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="2100" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -661,21 +661,21 @@
         <v>15</v>
       </c>
       <c r="B7" s="6">
-        <v>1071.9000000000001</v>
+        <v>1070</v>
       </c>
       <c r="C7" s="5">
         <v>100</v>
       </c>
       <c r="D7" s="8">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="F7" s="5">
         <f>B7*E7</f>
-        <v>1071.9000000000001</v>
+        <v>1114.5833333333335</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -683,21 +683,21 @@
         <v>16</v>
       </c>
       <c r="B8" s="6">
-        <v>1083.3</v>
+        <v>1070</v>
       </c>
       <c r="C8" s="6">
         <v>100</v>
       </c>
       <c r="D8" s="7">
-        <v>99.9</v>
+        <v>100.5</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ref="E8:E10" si="2">C8/D8</f>
-        <v>1.0010010010010009</v>
+        <v>0.99502487562189057</v>
       </c>
       <c r="F8" s="6">
         <f>B8*E8</f>
-        <v>1084.3843843843842</v>
+        <v>1064.676616915423</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -705,21 +705,21 @@
         <v>17</v>
       </c>
       <c r="B9" s="6">
-        <v>1072.3</v>
+        <v>1070</v>
       </c>
       <c r="C9" s="6">
         <v>100</v>
       </c>
       <c r="D9" s="7">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="2"/>
-        <v>1.0101010101010102</v>
+        <v>0.98039215686274506</v>
       </c>
       <c r="F9" s="6">
         <f>B9*E9</f>
-        <v>1083.1313131313132</v>
+        <v>1049.0196078431372</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -727,21 +727,21 @@
         <v>18</v>
       </c>
       <c r="B10" s="6">
-        <v>1088.7</v>
+        <v>1070</v>
       </c>
       <c r="C10" s="6">
         <v>100</v>
       </c>
       <c r="D10" s="7">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>0.99009900990099009</v>
+        <v>1.0526315789473684</v>
       </c>
       <c r="F10" s="6">
         <f>B10*E10</f>
-        <v>1077.920792079208</v>
+        <v>1126.3157894736842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>